<commit_message>
Actualización EXCEL Mesas de examen Septiembre 2018.
</commit_message>
<xml_diff>
--- a/03. Analisis y diseño/04. Base de datos/04. Archivos/tempus_mesas_sep18.xlsx
+++ b/03. Analisis y diseño/04. Base de datos/04. Archivos/tempus_mesas_sep18.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="190">
   <si>
     <t>Matemática I</t>
   </si>
@@ -278,6 +278,312 @@
   </si>
   <si>
     <t>Perroni</t>
+  </si>
+  <si>
+    <t>Introduccion Al Conocimiento Cientifico</t>
+  </si>
+  <si>
+    <t>Logica</t>
+  </si>
+  <si>
+    <t>Aprendizaje</t>
+  </si>
+  <si>
+    <t>Algebra Lineal</t>
+  </si>
+  <si>
+    <t>Probabilidades</t>
+  </si>
+  <si>
+    <t>Idioma Moderno Ingles</t>
+  </si>
+  <si>
+    <t>Enseñanza Y Curriculum</t>
+  </si>
+  <si>
+    <t>Estructuras Algebraicas</t>
+  </si>
+  <si>
+    <t>Estadistica</t>
+  </si>
+  <si>
+    <t>Fundamentos E Historia De Las Matematicas</t>
+  </si>
+  <si>
+    <t>Teoria De Grafos Y Progamacion Lineal</t>
+  </si>
+  <si>
+    <t>Taller De Practica Docente</t>
+  </si>
+  <si>
+    <t>Calculo Numerico</t>
+  </si>
+  <si>
+    <t>Pac</t>
+  </si>
+  <si>
+    <t>Castillo C.</t>
+  </si>
+  <si>
+    <t>Draghi</t>
+  </si>
+  <si>
+    <t>Paiva P.</t>
+  </si>
+  <si>
+    <t>Saldivia</t>
+  </si>
+  <si>
+    <t>Restivo</t>
+  </si>
+  <si>
+    <t>Rosales K.</t>
+  </si>
+  <si>
+    <t>Maglione D.</t>
+  </si>
+  <si>
+    <t>Saenz J. L.</t>
+  </si>
+  <si>
+    <t>Forchino</t>
+  </si>
+  <si>
+    <t>Diaz Mass S.</t>
+  </si>
+  <si>
+    <t>Segovia S.</t>
+  </si>
+  <si>
+    <t>Sanchez A.</t>
+  </si>
+  <si>
+    <t>Laje</t>
+  </si>
+  <si>
+    <t>Tacul E.</t>
+  </si>
+  <si>
+    <t>Damasio</t>
+  </si>
+  <si>
+    <t>Ivanissevich</t>
+  </si>
+  <si>
+    <t>Paiva</t>
+  </si>
+  <si>
+    <t>Naguil</t>
+  </si>
+  <si>
+    <t>Saldivia F.</t>
+  </si>
+  <si>
+    <t>Paulette M.</t>
+  </si>
+  <si>
+    <t>Hernandez S.</t>
+  </si>
+  <si>
+    <t>Ingenieria Química</t>
+  </si>
+  <si>
+    <t>Quimica General</t>
+  </si>
+  <si>
+    <t>Operaciones Unitarias III</t>
+  </si>
+  <si>
+    <t>Análisis Matemático I</t>
+  </si>
+  <si>
+    <t>Análisis Matemático II</t>
+  </si>
+  <si>
+    <t>Análisis Matemático III</t>
+  </si>
+  <si>
+    <t>Fisica II</t>
+  </si>
+  <si>
+    <t>Química Analitica I</t>
+  </si>
+  <si>
+    <t>Fisicoquimica</t>
+  </si>
+  <si>
+    <t>Estadistica Aplicada</t>
+  </si>
+  <si>
+    <t>Economia Y Organización Industrial</t>
+  </si>
+  <si>
+    <t>Operaciones Unitarias II</t>
+  </si>
+  <si>
+    <t>Operaciones Unitarias I</t>
+  </si>
+  <si>
+    <t>Tecnologia De Materiales Y Mecanica</t>
+  </si>
+  <si>
+    <t>Olivares F.</t>
+  </si>
+  <si>
+    <t>Blasich</t>
+  </si>
+  <si>
+    <t>Caminos</t>
+  </si>
+  <si>
+    <t>Palacios D.</t>
+  </si>
+  <si>
+    <t>Burgos</t>
+  </si>
+  <si>
+    <t>Laurlund C.</t>
+  </si>
+  <si>
+    <t>Villanueva L.</t>
+  </si>
+  <si>
+    <t>Quiroga J.</t>
+  </si>
+  <si>
+    <t>Mansilla N.</t>
+  </si>
+  <si>
+    <t>Pajares</t>
+  </si>
+  <si>
+    <t>Escalada J. P.</t>
+  </si>
+  <si>
+    <t>Sandoval</t>
+  </si>
+  <si>
+    <t>Cornaglia</t>
+  </si>
+  <si>
+    <t>Contingiani</t>
+  </si>
+  <si>
+    <t>Analista De Sistemas</t>
+  </si>
+  <si>
+    <t>Profesorado En Matemática</t>
+  </si>
+  <si>
+    <t>Ciencia Universidad Y Sociedad</t>
+  </si>
+  <si>
+    <t>Algebra</t>
+  </si>
+  <si>
+    <t>Procesos De Desarrollo De Software</t>
+  </si>
+  <si>
+    <t>Requerimientos De Software</t>
+  </si>
+  <si>
+    <t>Estructura De Datos</t>
+  </si>
+  <si>
+    <t>Análisis Y Diseño De Software</t>
+  </si>
+  <si>
+    <t>Validacion Y Verificacion De Software</t>
+  </si>
+  <si>
+    <t>Estadistica II</t>
+  </si>
+  <si>
+    <t>Sistemas Operativos Distribuidos</t>
+  </si>
+  <si>
+    <t>Programación Logica Y Funcional</t>
+  </si>
+  <si>
+    <t>Laboratorio De Desarrollo De Software</t>
+  </si>
+  <si>
+    <t>Licenciatura En Sistemas</t>
+  </si>
+  <si>
+    <t>Jaremchuk</t>
+  </si>
+  <si>
+    <t>Vilaboa</t>
+  </si>
+  <si>
+    <t>Carcamo Y.</t>
+  </si>
+  <si>
+    <t>Musci C.</t>
+  </si>
+  <si>
+    <t>Gentili</t>
+  </si>
+  <si>
+    <t>Laguia</t>
+  </si>
+  <si>
+    <t>Hallar</t>
+  </si>
+  <si>
+    <t>Farias R.</t>
+  </si>
+  <si>
+    <t>Gesto E.</t>
+  </si>
+  <si>
+    <t>Gonzalez L.</t>
+  </si>
+  <si>
+    <t>Reinaga H.</t>
+  </si>
+  <si>
+    <t>Gonzalez D.</t>
+  </si>
+  <si>
+    <t>Vidal</t>
+  </si>
+  <si>
+    <t>Saldivia C.</t>
+  </si>
+  <si>
+    <t>Millado P.</t>
+  </si>
+  <si>
+    <t>Sofia O.</t>
+  </si>
+  <si>
+    <t>Soto H.</t>
+  </si>
+  <si>
+    <t>Livacic C.</t>
+  </si>
+  <si>
+    <t>Talay A.</t>
+  </si>
+  <si>
+    <t>Sierpe L.</t>
+  </si>
+  <si>
+    <t>Laguia D.</t>
+  </si>
+  <si>
+    <t>Hallar K.</t>
+  </si>
+  <si>
+    <t>Casas S.</t>
+  </si>
+  <si>
+    <t>Enriquez J.</t>
+  </si>
+  <si>
+    <t>Miranda M.</t>
   </si>
 </sst>
 </file>
@@ -313,10 +619,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,21 +928,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I24"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="D59" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -1196,7 +1505,1299 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I25" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I26" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I27" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I28" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" t="s">
+        <v>110</v>
+      </c>
+      <c r="H29" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I29" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" t="s">
+        <v>113</v>
+      </c>
+      <c r="H30" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I30" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" t="s">
+        <v>114</v>
+      </c>
+      <c r="E31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" t="s">
+        <v>103</v>
+      </c>
+      <c r="H32" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I32" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" t="s">
+        <v>108</v>
+      </c>
+      <c r="H33" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I33" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" t="s">
+        <v>118</v>
+      </c>
+      <c r="H34" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I34" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" t="s">
+        <v>119</v>
+      </c>
+      <c r="H35" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I35" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I36" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F37" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I37" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" t="s">
+        <v>138</v>
+      </c>
+      <c r="H38" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I38" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" t="s">
+        <v>140</v>
+      </c>
+      <c r="H39" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I39" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" t="s">
+        <v>126</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>142</v>
+      </c>
+      <c r="G40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I40" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" t="s">
+        <v>143</v>
+      </c>
+      <c r="E41" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" t="s">
+        <v>110</v>
+      </c>
+      <c r="H41" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I41" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>142</v>
+      </c>
+      <c r="H42" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I42" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>123</v>
+      </c>
+      <c r="C43" t="s">
+        <v>129</v>
+      </c>
+      <c r="D43" t="s">
+        <v>58</v>
+      </c>
+      <c r="E43" t="s">
+        <v>59</v>
+      </c>
+      <c r="F43" t="s">
+        <v>144</v>
+      </c>
+      <c r="G43" t="s">
+        <v>60</v>
+      </c>
+      <c r="H43" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I43" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" t="s">
+        <v>145</v>
+      </c>
+      <c r="H44" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" t="s">
+        <v>112</v>
+      </c>
+      <c r="H45" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I45" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="C46" t="s">
+        <v>131</v>
+      </c>
+      <c r="D46" t="s">
+        <v>146</v>
+      </c>
+      <c r="E46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F46" t="s">
+        <v>144</v>
+      </c>
+      <c r="H46" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I46" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C47" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47" t="s">
+        <v>148</v>
+      </c>
+      <c r="H47" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I47" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" t="s">
+        <v>84</v>
+      </c>
+      <c r="F48" t="s">
+        <v>85</v>
+      </c>
+      <c r="H48" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I48" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" t="s">
+        <v>35</v>
+      </c>
+      <c r="E49" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" t="s">
+        <v>150</v>
+      </c>
+      <c r="H49" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I49" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" t="s">
+        <v>134</v>
+      </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E50" t="s">
+        <v>140</v>
+      </c>
+      <c r="F50" t="s">
+        <v>150</v>
+      </c>
+      <c r="H50" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I50" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H51" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I51" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>16</v>
+      </c>
+      <c r="B52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
+        <v>165</v>
+      </c>
+      <c r="E52" t="s">
+        <v>166</v>
+      </c>
+      <c r="F52" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52" t="s">
+        <v>168</v>
+      </c>
+      <c r="H52" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I52" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>16</v>
+      </c>
+      <c r="B53" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" t="s">
+        <v>119</v>
+      </c>
+      <c r="E53" t="s">
+        <v>169</v>
+      </c>
+      <c r="F53" t="s">
+        <v>60</v>
+      </c>
+      <c r="H53" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I53" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>16</v>
+      </c>
+      <c r="B54" t="s">
+        <v>151</v>
+      </c>
+      <c r="C54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" t="s">
+        <v>170</v>
+      </c>
+      <c r="E54" t="s">
+        <v>171</v>
+      </c>
+      <c r="F54" t="s">
+        <v>172</v>
+      </c>
+      <c r="H54" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I54" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>16</v>
+      </c>
+      <c r="B55" t="s">
+        <v>151</v>
+      </c>
+      <c r="C55" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I55" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>16</v>
+      </c>
+      <c r="B56" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" t="s">
+        <v>156</v>
+      </c>
+      <c r="D56" t="s">
+        <v>171</v>
+      </c>
+      <c r="E56" t="s">
+        <v>173</v>
+      </c>
+      <c r="F56" t="s">
+        <v>174</v>
+      </c>
+      <c r="H56" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I56" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>16</v>
+      </c>
+      <c r="B57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" t="s">
+        <v>157</v>
+      </c>
+      <c r="D57" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" t="s">
+        <v>176</v>
+      </c>
+      <c r="F57" t="s">
+        <v>177</v>
+      </c>
+      <c r="G57" t="s">
+        <v>178</v>
+      </c>
+      <c r="H57" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I57" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>16</v>
+      </c>
+      <c r="B58" t="s">
+        <v>151</v>
+      </c>
+      <c r="C58" t="s">
+        <v>158</v>
+      </c>
+      <c r="D58" t="s">
+        <v>185</v>
+      </c>
+      <c r="E58" t="s">
+        <v>179</v>
+      </c>
+      <c r="F58" t="s">
+        <v>186</v>
+      </c>
+      <c r="G58" t="s">
+        <v>180</v>
+      </c>
+      <c r="H58" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I58" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>16</v>
+      </c>
+      <c r="B59" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" t="s">
+        <v>159</v>
+      </c>
+      <c r="D59" t="s">
+        <v>185</v>
+      </c>
+      <c r="E59" t="s">
+        <v>179</v>
+      </c>
+      <c r="F59" t="s">
+        <v>186</v>
+      </c>
+      <c r="G59" t="s">
+        <v>180</v>
+      </c>
+      <c r="H59" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I59" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>16</v>
+      </c>
+      <c r="B60" t="s">
+        <v>151</v>
+      </c>
+      <c r="C60" t="s">
+        <v>160</v>
+      </c>
+      <c r="D60" t="s">
+        <v>109</v>
+      </c>
+      <c r="E60" t="s">
+        <v>110</v>
+      </c>
+      <c r="F60" t="s">
+        <v>148</v>
+      </c>
+      <c r="G60" t="s">
+        <v>149</v>
+      </c>
+      <c r="H60" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I60" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>16</v>
+      </c>
+      <c r="B61" t="s">
+        <v>151</v>
+      </c>
+      <c r="C61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D61" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" t="s">
+        <v>184</v>
+      </c>
+      <c r="F61" t="s">
+        <v>183</v>
+      </c>
+      <c r="G61" t="s">
+        <v>182</v>
+      </c>
+      <c r="H61" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I61" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>16</v>
+      </c>
+      <c r="B62" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" t="s">
+        <v>188</v>
+      </c>
+      <c r="F62" t="s">
+        <v>178</v>
+      </c>
+      <c r="G62" t="s">
+        <v>189</v>
+      </c>
+      <c r="H62" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I62" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D63" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" t="s">
+        <v>184</v>
+      </c>
+      <c r="F63" t="s">
+        <v>183</v>
+      </c>
+      <c r="G63" t="s">
+        <v>182</v>
+      </c>
+      <c r="H63" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I63" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>72</v>
+      </c>
+      <c r="B64" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" t="s">
+        <v>153</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H64" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I64" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>72</v>
+      </c>
+      <c r="B65" t="s">
+        <v>164</v>
+      </c>
+      <c r="C65" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I65" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>72</v>
+      </c>
+      <c r="B66" t="s">
+        <v>164</v>
+      </c>
+      <c r="C66" t="s">
+        <v>155</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I66" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>72</v>
+      </c>
+      <c r="B67" t="s">
+        <v>164</v>
+      </c>
+      <c r="C67" t="s">
+        <v>126</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I67" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>72</v>
+      </c>
+      <c r="B68" t="s">
+        <v>164</v>
+      </c>
+      <c r="C68" t="s">
+        <v>156</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G68" s="3"/>
+      <c r="H68" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I68" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
+        <v>164</v>
+      </c>
+      <c r="C69" t="s">
+        <v>157</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H69" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I69" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>72</v>
+      </c>
+      <c r="B70" t="s">
+        <v>164</v>
+      </c>
+      <c r="C70" t="s">
+        <v>158</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H70" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I70" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" t="s">
+        <v>159</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="H71" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I71" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>164</v>
+      </c>
+      <c r="C72" t="s">
+        <v>160</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H72" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I72" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+      <c r="C73" t="s">
+        <v>161</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H73" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I73" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>164</v>
+      </c>
+      <c r="C74" t="s">
+        <v>162</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H74" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I74" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" t="s">
+        <v>163</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="H75" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I75" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización EXCEL Mesas de examen Septiembre 2018. Eliminación archivos duplicados.
</commit_message>
<xml_diff>
--- a/03. Analisis y diseño/04. Base de datos/04. Archivos/tempus_mesas_sep18.xlsx
+++ b/03. Analisis y diseño/04. Base de datos/04. Archivos/tempus_mesas_sep18.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="406">
   <si>
     <t>Matemática I</t>
   </si>
@@ -886,9 +886,6 @@
     <t>Ingles III</t>
   </si>
   <si>
-    <t>Tecnicatura En Turismo</t>
-  </si>
-  <si>
     <t>Vilaboa J.</t>
   </si>
   <si>
@@ -983,6 +980,258 @@
   </si>
   <si>
     <t>Agüero A.</t>
+  </si>
+  <si>
+    <t>Nivel De Ofimatica</t>
+  </si>
+  <si>
+    <t>Higiene Y Seguridad Industrial</t>
+  </si>
+  <si>
+    <t>Economia I</t>
+  </si>
+  <si>
+    <t>Calculo Financiero</t>
+  </si>
+  <si>
+    <t>Gestion De La Calidad</t>
+  </si>
+  <si>
+    <t>Administracion II</t>
+  </si>
+  <si>
+    <t>Sistemas Contables I</t>
+  </si>
+  <si>
+    <t>Sistemas Contables II</t>
+  </si>
+  <si>
+    <t>Tecnica  Impositiva</t>
+  </si>
+  <si>
+    <t>Constanzo</t>
+  </si>
+  <si>
+    <t>Aguirre M.</t>
+  </si>
+  <si>
+    <t>Miranda</t>
+  </si>
+  <si>
+    <t>Martinez LL.</t>
+  </si>
+  <si>
+    <t>Coloe</t>
+  </si>
+  <si>
+    <t>Maraschin</t>
+  </si>
+  <si>
+    <t>Garcia R.</t>
+  </si>
+  <si>
+    <t>Duran Peralta</t>
+  </si>
+  <si>
+    <t>Borroni</t>
+  </si>
+  <si>
+    <t>Muñiz</t>
+  </si>
+  <si>
+    <t>Zunino</t>
+  </si>
+  <si>
+    <t>Matematica I</t>
+  </si>
+  <si>
+    <t>Derecho Empresarial I</t>
+  </si>
+  <si>
+    <t>Derecho Empresarial II</t>
+  </si>
+  <si>
+    <t>Economia II</t>
+  </si>
+  <si>
+    <t>Costos</t>
+  </si>
+  <si>
+    <t>Comercializacion I</t>
+  </si>
+  <si>
+    <t>Comercializacion II</t>
+  </si>
+  <si>
+    <t>Administracion Financiera</t>
+  </si>
+  <si>
+    <t>Modelos De Decision</t>
+  </si>
+  <si>
+    <t>Administracion III</t>
+  </si>
+  <si>
+    <t>Licenciatura En Administración</t>
+  </si>
+  <si>
+    <t>Schinelli</t>
+  </si>
+  <si>
+    <t>Hallar Z.</t>
+  </si>
+  <si>
+    <t>Fernandez T.</t>
+  </si>
+  <si>
+    <t>Miranda G.</t>
+  </si>
+  <si>
+    <t>Barahona</t>
+  </si>
+  <si>
+    <t>Profesorado En Economia Y Gestión De Organizaciones</t>
+  </si>
+  <si>
+    <t>Tecnicatura Universitaria En Gestión De Organizaciones</t>
+  </si>
+  <si>
+    <t>Licenciatura En Psicopedagogía</t>
+  </si>
+  <si>
+    <t>Teoria Psicosocial</t>
+  </si>
+  <si>
+    <t>Seminario Nec. Educativas Especiales</t>
+  </si>
+  <si>
+    <t>Educacion Formal II</t>
+  </si>
+  <si>
+    <t>Seminario Psicosociolinguistico</t>
+  </si>
+  <si>
+    <t>Problemática En Salud</t>
+  </si>
+  <si>
+    <t>Teoria y Met. De La Inv. En Ciencias Sociales</t>
+  </si>
+  <si>
+    <t>Seminario De Analisis Institucional</t>
+  </si>
+  <si>
+    <t>Seminario De Familia</t>
+  </si>
+  <si>
+    <t>Educacion Formal I</t>
+  </si>
+  <si>
+    <t>Teoria Psicoanalitica</t>
+  </si>
+  <si>
+    <t>Rodriguez G.</t>
+  </si>
+  <si>
+    <t>Montane J.</t>
+  </si>
+  <si>
+    <t>Cornejo P.</t>
+  </si>
+  <si>
+    <t>Stetler L.</t>
+  </si>
+  <si>
+    <t>Reinoso M.</t>
+  </si>
+  <si>
+    <t>Cruz Z.</t>
+  </si>
+  <si>
+    <t>Sanchez C.</t>
+  </si>
+  <si>
+    <t>Torea A.</t>
+  </si>
+  <si>
+    <t>Gonzalez C.</t>
+  </si>
+  <si>
+    <t>Michniuk</t>
+  </si>
+  <si>
+    <t>Patzi</t>
+  </si>
+  <si>
+    <t>Martinez T.</t>
+  </si>
+  <si>
+    <t>Psicopatologia</t>
+  </si>
+  <si>
+    <t>Clinica Psicopedagogica II</t>
+  </si>
+  <si>
+    <t>Seminario De Analisis De La Practica Profesional</t>
+  </si>
+  <si>
+    <t>Fundamentos Bioneurologicos Del Aprendizaje</t>
+  </si>
+  <si>
+    <t>Neuropsiquiatria</t>
+  </si>
+  <si>
+    <t>Seminario De Introduccion A La PSP</t>
+  </si>
+  <si>
+    <t>Practica Profesional</t>
+  </si>
+  <si>
+    <t>Residencia Profesional</t>
+  </si>
+  <si>
+    <t>Patzi M.</t>
+  </si>
+  <si>
+    <t>San Roman A.</t>
+  </si>
+  <si>
+    <t>Filippo M.</t>
+  </si>
+  <si>
+    <t>Fernandez D.</t>
+  </si>
+  <si>
+    <t>Romano C.</t>
+  </si>
+  <si>
+    <t>Bonotto</t>
+  </si>
+  <si>
+    <t>Diaz M.</t>
+  </si>
+  <si>
+    <t>Arias P.</t>
+  </si>
+  <si>
+    <t>Novack</t>
+  </si>
+  <si>
+    <t>Silva A.</t>
+  </si>
+  <si>
+    <t>Analisis Politico Y Organización Del Sistema Educativo</t>
+  </si>
+  <si>
+    <t>Teorias Del Aprendizaje</t>
+  </si>
+  <si>
+    <t>Seminario De Investigacion PSP</t>
+  </si>
+  <si>
+    <t>Stettler</t>
+  </si>
+  <si>
+    <t>Tecnicatura Universitaria En Turismo</t>
   </si>
 </sst>
 </file>
@@ -1018,11 +1267,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,16 +1577,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I167"/>
+  <dimension ref="A1:I253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B253" sqref="B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -1345,7 +1595,10 @@
     <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>23</v>
+      </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -1371,7 +1624,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>23</v>
+      </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1394,7 +1650,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>23</v>
+      </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1420,7 +1679,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>23</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1708,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>23</v>
+      </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1469,7 +1734,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>23</v>
+      </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1495,7 +1763,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>23</v>
+      </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1789,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>23</v>
+      </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -1541,7 +1815,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>23</v>
+      </c>
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -1567,7 +1844,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>23</v>
+      </c>
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -1590,7 +1870,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>23</v>
+      </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -1613,7 +1896,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>23</v>
+      </c>
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1636,7 +1922,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>23</v>
+      </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
@@ -1659,7 +1948,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>23</v>
+      </c>
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -1682,7 +1974,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>23</v>
+      </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
@@ -1705,7 +2000,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>23</v>
+      </c>
       <c r="B16" t="s">
         <v>3</v>
       </c>
@@ -1728,7 +2026,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>23</v>
+      </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1751,7 +2052,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>23</v>
+      </c>
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -1774,7 +2078,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>23</v>
+      </c>
       <c r="B19" t="s">
         <v>3</v>
       </c>
@@ -1794,7 +2101,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>23</v>
+      </c>
       <c r="B20" t="s">
         <v>3</v>
       </c>
@@ -1817,7 +2127,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>23</v>
+      </c>
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1837,7 +2150,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23</v>
+      </c>
       <c r="B22" t="s">
         <v>3</v>
       </c>
@@ -1857,7 +2173,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
       <c r="B23" t="s">
         <v>3</v>
       </c>
@@ -1880,7 +2199,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
       <c r="B24" t="s">
         <v>3</v>
       </c>
@@ -1903,7 +2225,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>49</v>
+      </c>
       <c r="B25" t="s">
         <v>152</v>
       </c>
@@ -1926,7 +2251,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>49</v>
+      </c>
       <c r="B26" s="3" t="s">
         <v>152</v>
       </c>
@@ -1949,7 +2277,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>49</v>
+      </c>
       <c r="B27" s="3" t="s">
         <v>152</v>
       </c>
@@ -1969,7 +2300,10 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>49</v>
+      </c>
       <c r="B28" s="3" t="s">
         <v>152</v>
       </c>
@@ -1992,7 +2326,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>49</v>
+      </c>
       <c r="B29" s="3" t="s">
         <v>152</v>
       </c>
@@ -2015,7 +2352,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>49</v>
+      </c>
       <c r="B30" s="3" t="s">
         <v>152</v>
       </c>
@@ -2038,7 +2378,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>49</v>
+      </c>
       <c r="B31" s="3" t="s">
         <v>152</v>
       </c>
@@ -2061,7 +2404,10 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>49</v>
+      </c>
       <c r="B32" s="3" t="s">
         <v>152</v>
       </c>
@@ -2084,7 +2430,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>49</v>
+      </c>
       <c r="B33" s="3" t="s">
         <v>152</v>
       </c>
@@ -2107,7 +2456,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>49</v>
+      </c>
       <c r="B34" s="3" t="s">
         <v>152</v>
       </c>
@@ -2130,7 +2482,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>49</v>
+      </c>
       <c r="B35" s="3" t="s">
         <v>152</v>
       </c>
@@ -2153,7 +2508,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>49</v>
+      </c>
       <c r="B36" s="3" t="s">
         <v>152</v>
       </c>
@@ -2176,7 +2534,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>49</v>
+      </c>
       <c r="B37" s="3" t="s">
         <v>152</v>
       </c>
@@ -2199,7 +2560,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>69</v>
+      </c>
       <c r="B38" t="s">
         <v>123</v>
       </c>
@@ -2225,7 +2589,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>69</v>
+      </c>
       <c r="B39" t="s">
         <v>123</v>
       </c>
@@ -2245,7 +2612,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>69</v>
+      </c>
       <c r="B40" t="s">
         <v>123</v>
       </c>
@@ -2271,7 +2641,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>69</v>
+      </c>
       <c r="B41" t="s">
         <v>123</v>
       </c>
@@ -2294,7 +2667,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>69</v>
+      </c>
       <c r="B42" t="s">
         <v>123</v>
       </c>
@@ -2314,7 +2690,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>69</v>
+      </c>
       <c r="B43" t="s">
         <v>123</v>
       </c>
@@ -2340,7 +2719,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>69</v>
+      </c>
       <c r="B44" t="s">
         <v>123</v>
       </c>
@@ -2360,7 +2742,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>69</v>
+      </c>
       <c r="B45" t="s">
         <v>123</v>
       </c>
@@ -2380,7 +2765,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>69</v>
+      </c>
       <c r="B46" t="s">
         <v>123</v>
       </c>
@@ -2403,7 +2791,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>69</v>
+      </c>
       <c r="B47" t="s">
         <v>123</v>
       </c>
@@ -2426,7 +2817,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>69</v>
+      </c>
       <c r="B48" t="s">
         <v>123</v>
       </c>
@@ -2450,6 +2844,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>69</v>
+      </c>
       <c r="B49" t="s">
         <v>123</v>
       </c>
@@ -2473,6 +2870,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>69</v>
+      </c>
       <c r="B50" t="s">
         <v>123</v>
       </c>
@@ -2496,6 +2896,9 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>69</v>
+      </c>
       <c r="B51" t="s">
         <v>123</v>
       </c>
@@ -3195,6 +3598,9 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>46</v>
+      </c>
       <c r="B76" s="3" t="s">
         <v>211</v>
       </c>
@@ -3221,6 +3627,9 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>46</v>
+      </c>
       <c r="B77" s="3" t="s">
         <v>211</v>
       </c>
@@ -3247,6 +3656,9 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>46</v>
+      </c>
       <c r="B78" s="3" t="s">
         <v>211</v>
       </c>
@@ -3273,6 +3685,9 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>46</v>
+      </c>
       <c r="B79" s="3" t="s">
         <v>211</v>
       </c>
@@ -3299,6 +3714,9 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>46</v>
+      </c>
       <c r="B80" s="3" t="s">
         <v>211</v>
       </c>
@@ -3321,7 +3739,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>46</v>
+      </c>
       <c r="B81" s="3" t="s">
         <v>211</v>
       </c>
@@ -3344,7 +3765,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>46</v>
+      </c>
       <c r="B82" t="s">
         <v>211</v>
       </c>
@@ -3370,7 +3794,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>47</v>
+      </c>
       <c r="B83" t="s">
         <v>210</v>
       </c>
@@ -3393,7 +3820,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>47</v>
+      </c>
       <c r="B84" t="s">
         <v>210</v>
       </c>
@@ -3413,7 +3843,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>47</v>
+      </c>
       <c r="B85" t="s">
         <v>210</v>
       </c>
@@ -3436,7 +3869,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>47</v>
+      </c>
       <c r="B86" t="s">
         <v>210</v>
       </c>
@@ -3456,7 +3892,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>47</v>
+      </c>
       <c r="B87" t="s">
         <v>210</v>
       </c>
@@ -3479,7 +3918,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>47</v>
+      </c>
       <c r="B88" t="s">
         <v>210</v>
       </c>
@@ -3505,7 +3947,10 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>47</v>
+      </c>
       <c r="B89" t="s">
         <v>210</v>
       </c>
@@ -3528,7 +3973,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>47</v>
+      </c>
       <c r="B90" t="s">
         <v>210</v>
       </c>
@@ -3548,7 +3996,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>1</v>
+      </c>
       <c r="B91" t="s">
         <v>234</v>
       </c>
@@ -3571,7 +4022,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>1</v>
+      </c>
       <c r="B92" t="s">
         <v>234</v>
       </c>
@@ -3591,7 +4045,10 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>1</v>
+      </c>
       <c r="B93" t="s">
         <v>234</v>
       </c>
@@ -3614,7 +4071,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1</v>
+      </c>
       <c r="B94" t="s">
         <v>234</v>
       </c>
@@ -3634,7 +4094,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>1</v>
+      </c>
       <c r="B95" t="s">
         <v>234</v>
       </c>
@@ -3654,7 +4117,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>1</v>
+      </c>
       <c r="B96" t="s">
         <v>234</v>
       </c>
@@ -3677,7 +4143,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>1</v>
+      </c>
       <c r="B97" t="s">
         <v>234</v>
       </c>
@@ -3700,7 +4169,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>1</v>
+      </c>
       <c r="B98" t="s">
         <v>234</v>
       </c>
@@ -3723,7 +4195,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>1</v>
+      </c>
       <c r="B99" t="s">
         <v>234</v>
       </c>
@@ -3743,7 +4218,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>1</v>
+      </c>
       <c r="B100" t="s">
         <v>234</v>
       </c>
@@ -3766,7 +4244,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>1</v>
+      </c>
       <c r="B101" t="s">
         <v>234</v>
       </c>
@@ -3786,7 +4267,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>1</v>
+      </c>
       <c r="B102" t="s">
         <v>234</v>
       </c>
@@ -3809,7 +4293,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>60</v>
+      </c>
       <c r="B103" t="s">
         <v>260</v>
       </c>
@@ -3832,7 +4319,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>60</v>
+      </c>
       <c r="B104" t="s">
         <v>260</v>
       </c>
@@ -3852,7 +4342,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>60</v>
+      </c>
       <c r="B105" t="s">
         <v>260</v>
       </c>
@@ -3872,7 +4365,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>60</v>
+      </c>
       <c r="B106" t="s">
         <v>260</v>
       </c>
@@ -3895,7 +4391,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>60</v>
+      </c>
       <c r="B107" t="s">
         <v>260</v>
       </c>
@@ -3918,7 +4417,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>60</v>
+      </c>
       <c r="B108" t="s">
         <v>260</v>
       </c>
@@ -3941,7 +4443,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>60</v>
+      </c>
       <c r="B109" t="s">
         <v>260</v>
       </c>
@@ -3961,7 +4466,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>60</v>
+      </c>
       <c r="B110" t="s">
         <v>260</v>
       </c>
@@ -3984,7 +4492,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>60</v>
+      </c>
       <c r="B111" t="s">
         <v>260</v>
       </c>
@@ -4004,7 +4515,10 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>60</v>
+      </c>
       <c r="B112" t="s">
         <v>260</v>
       </c>
@@ -4027,7 +4541,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>4</v>
+      </c>
       <c r="B113" t="s">
         <v>267</v>
       </c>
@@ -4050,7 +4567,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>4</v>
+      </c>
       <c r="B114" t="s">
         <v>267</v>
       </c>
@@ -4073,7 +4593,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>4</v>
+      </c>
       <c r="B115" t="s">
         <v>267</v>
       </c>
@@ -4096,7 +4619,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>4</v>
+      </c>
       <c r="B116" t="s">
         <v>267</v>
       </c>
@@ -4119,7 +4645,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>4</v>
+      </c>
       <c r="B117" t="s">
         <v>267</v>
       </c>
@@ -4142,7 +4671,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>4</v>
+      </c>
       <c r="B118" t="s">
         <v>267</v>
       </c>
@@ -4165,7 +4697,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>4</v>
+      </c>
       <c r="B119" t="s">
         <v>267</v>
       </c>
@@ -4188,7 +4723,10 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>64</v>
+      </c>
       <c r="B120" t="s">
         <v>272</v>
       </c>
@@ -4211,7 +4749,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>64</v>
+      </c>
       <c r="B121" s="3" t="s">
         <v>272</v>
       </c>
@@ -4234,7 +4775,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>64</v>
+      </c>
       <c r="B122" s="3" t="s">
         <v>272</v>
       </c>
@@ -4257,7 +4801,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>64</v>
+      </c>
       <c r="B123" s="3" t="s">
         <v>272</v>
       </c>
@@ -4280,7 +4827,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>64</v>
+      </c>
       <c r="B124" s="3" t="s">
         <v>272</v>
       </c>
@@ -4303,7 +4853,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>64</v>
+      </c>
       <c r="B125" s="3" t="s">
         <v>272</v>
       </c>
@@ -4326,7 +4879,10 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>64</v>
+      </c>
       <c r="B126" s="3" t="s">
         <v>272</v>
       </c>
@@ -4349,15 +4905,18 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>62</v>
+      </c>
       <c r="B127" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>153</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E127" s="3" t="s">
         <v>165</v>
@@ -4375,9 +4934,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>62</v>
+      </c>
       <c r="B128" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>268</v>
@@ -4389,7 +4951,7 @@
         <v>282</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H128" s="1">
         <v>43370</v>
@@ -4398,18 +4960,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>62</v>
+      </c>
       <c r="B129" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>269</v>
       </c>
       <c r="D129" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E129" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="E129" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="H129" s="1">
         <v>43368</v>
@@ -4418,18 +4983,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>62</v>
+      </c>
       <c r="B130" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>270</v>
       </c>
       <c r="D130" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E130" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="E130" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="H130" s="1">
         <v>43367</v>
@@ -4438,18 +5006,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>62</v>
+      </c>
       <c r="B131" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>271</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H131" s="1">
         <v>43367</v>
@@ -4458,21 +5029,24 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>62</v>
+      </c>
       <c r="B132" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>285</v>
       </c>
       <c r="D132" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E132" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E132" s="3" t="s">
-        <v>293</v>
-      </c>
       <c r="F132" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H132" s="1">
         <v>43367</v>
@@ -4481,15 +5055,18 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>62</v>
+      </c>
       <c r="B133" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>286</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E133" s="3" t="s">
         <v>143</v>
@@ -4504,9 +5081,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>62</v>
+      </c>
       <c r="B134" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>287</v>
@@ -4527,9 +5107,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>62</v>
+      </c>
       <c r="B135" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>288</v>
@@ -4547,9 +5130,12 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>62</v>
+      </c>
       <c r="B136" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>289</v>
@@ -4567,9 +5153,12 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>62</v>
+      </c>
       <c r="B137" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>1</v>
@@ -4593,18 +5182,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>62</v>
+      </c>
       <c r="B138" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D138" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E138" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>303</v>
       </c>
       <c r="H138" s="1">
         <v>43369</v>
@@ -4613,12 +5205,15 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>62</v>
+      </c>
       <c r="B139" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D139" s="3" t="s">
         <v>205</v>
@@ -4636,18 +5231,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>62</v>
+      </c>
       <c r="B140" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D140" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H140" s="1">
         <v>43369</v>
@@ -4656,18 +5254,21 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>62</v>
+      </c>
       <c r="B141" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D141" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H141" s="1">
         <v>43368</v>
@@ -4676,18 +5277,21 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>62</v>
+      </c>
       <c r="B142" s="3" t="s">
-        <v>290</v>
+        <v>405</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D142" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H142" s="1">
         <v>43368</v>
@@ -4696,15 +5300,18 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>61</v>
+      </c>
       <c r="B143" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>153</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E143" s="3" t="s">
         <v>165</v>
@@ -4722,9 +5329,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>61</v>
+      </c>
       <c r="B144" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>268</v>
@@ -4736,7 +5346,7 @@
         <v>282</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H144" s="1">
         <v>43370</v>
@@ -4745,18 +5355,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="145" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>61</v>
+      </c>
       <c r="B145" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>269</v>
       </c>
       <c r="D145" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E145" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="H145" s="1">
         <v>43368</v>
@@ -4765,18 +5378,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>61</v>
+      </c>
       <c r="B146" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>270</v>
       </c>
       <c r="D146" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E146" s="3" t="s">
         <v>292</v>
-      </c>
-      <c r="E146" s="3" t="s">
-        <v>293</v>
       </c>
       <c r="H146" s="1">
         <v>43367</v>
@@ -4785,18 +5401,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="147" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>61</v>
+      </c>
       <c r="B147" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>271</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H147" s="1">
         <v>43367</v>
@@ -4805,21 +5424,24 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="148" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>61</v>
+      </c>
       <c r="B148" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>285</v>
       </c>
       <c r="D148" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E148" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="E148" s="3" t="s">
-        <v>293</v>
-      </c>
       <c r="F148" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H148" s="1">
         <v>43367</v>
@@ -4828,15 +5450,18 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="149" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>61</v>
+      </c>
       <c r="B149" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>286</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E149" s="3" t="s">
         <v>143</v>
@@ -4851,9 +5476,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>61</v>
+      </c>
       <c r="B150" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>287</v>
@@ -4874,9 +5502,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="151" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>61</v>
+      </c>
       <c r="B151" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>288</v>
@@ -4894,9 +5525,12 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="152" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>61</v>
+      </c>
       <c r="B152" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C152" s="3" t="s">
         <v>289</v>
@@ -4914,9 +5548,12 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="153" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>61</v>
+      </c>
       <c r="B153" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C153" s="3" t="s">
         <v>1</v>
@@ -4940,18 +5577,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>61</v>
+      </c>
       <c r="B154" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D154" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E154" s="3" t="s">
         <v>302</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>303</v>
       </c>
       <c r="H154" s="1">
         <v>43369</v>
@@ -4960,12 +5600,15 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="155" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>61</v>
+      </c>
       <c r="B155" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>205</v>
@@ -4983,18 +5626,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>61</v>
+      </c>
       <c r="B156" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H156" s="1">
         <v>43368</v>
@@ -5003,18 +5649,21 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="157" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>61</v>
+      </c>
       <c r="B157" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H157" s="1">
         <v>43368</v>
@@ -5023,9 +5672,12 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="158" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>918</v>
+      </c>
       <c r="B158" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>190</v>
@@ -5046,21 +5698,24 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="159" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>918</v>
+      </c>
       <c r="B159" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>306</v>
-      </c>
-      <c r="C159" s="3" t="s">
-        <v>307</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>256</v>
       </c>
       <c r="E159" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="F159" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="F159" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="H159" s="1">
         <v>43371</v>
@@ -5069,21 +5724,24 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="160" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>918</v>
+      </c>
       <c r="B160" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>256</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H160" s="1">
         <v>43371</v>
@@ -5092,18 +5750,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>918</v>
+      </c>
       <c r="B161" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D161" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="E161" s="3" t="s">
         <v>316</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>317</v>
       </c>
       <c r="H161" s="1">
         <v>43371</v>
@@ -5112,15 +5773,18 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="162" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>918</v>
+      </c>
       <c r="B162" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>153</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E162" s="3" t="s">
         <v>165</v>
@@ -5138,18 +5802,21 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="163" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>918</v>
+      </c>
       <c r="B163" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F163" s="3" t="s">
         <v>168</v>
@@ -5161,9 +5828,12 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>918</v>
+      </c>
       <c r="B164" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>88</v>
@@ -5184,12 +5854,15 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>918</v>
+      </c>
       <c r="B165" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D165" s="3" t="s">
         <v>111</v>
@@ -5205,18 +5878,21 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>918</v>
+      </c>
       <c r="B166" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D166" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E166" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="H166" s="1">
         <v>43369</v>
@@ -5225,27 +5901,2221 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>918</v>
+      </c>
       <c r="B167" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C167" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="E167" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D167" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="E167" s="3" t="s">
+      <c r="F167" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="F167" s="3" t="s">
-        <v>315</v>
       </c>
       <c r="H167" s="1">
         <v>43371</v>
       </c>
       <c r="I167" s="2">
         <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>913</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H168" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I168" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>913</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H169" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I169" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>913</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H170" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I170" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>913</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="H171" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I171" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>913</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H172" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I172" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>913</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H173" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I173" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>913</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H174" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I174" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>913</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H175" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I175" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>913</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H176" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I176" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>913</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H177" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I177" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>913</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H178" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I178" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>913</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H179" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I179" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>913</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H180" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I180" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>913</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H181" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I181" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>913</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H182" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I182" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>913</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H183" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I183" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>913</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H184" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I184" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>913</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H185" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I185" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>913</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H186" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I186" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>913</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H187" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I187" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>913</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="H188" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I188" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>913</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H189" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I189" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>913</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="H190" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I190" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>914</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G191" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H191" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I191" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>914</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H192" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I192" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>914</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="H193" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I193" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>914</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H194" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I194" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>914</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D195" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E195" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H195" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I195" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>914</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D196" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E196" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H196" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I196" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>914</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E197" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H197" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I197" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>914</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D198" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E198" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H198" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I198" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>914</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E199" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F199" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H199" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I199" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>914</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H200" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I200" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>914</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H201" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I201" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>914</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H202" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I202" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>914</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H203" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I203" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>914</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E204" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H204" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I204" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>914</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E205" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F205" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H205" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I205" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>914</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H206" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I206" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>914</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E207" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H207" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I207" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>912</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E208" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G208" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="H208" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I208" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>912</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E209" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F209" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G209" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H209" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I209" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>912</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E210" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="H210" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I210" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>912</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E211" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="F211" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H211" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I211" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>912</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H212" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I212" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>912</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E213" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F213" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H213" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I213" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>912</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E214" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H214" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I214" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>912</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E215" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H215" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I215" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>912</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E216" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H216" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I216" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>912</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E217" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F217" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="H217" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I217" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>912</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="F218" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="H218" s="1">
+        <v>43376</v>
+      </c>
+      <c r="I218" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>912</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E219" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F219" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H219" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I219" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>912</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E220" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H220" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I220" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>912</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E221" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H221" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I221" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>912</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E222" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F222" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H222" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I222" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>912</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E223" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F223" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H223" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I223" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>45</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G224" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H224" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I224" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>45</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E225" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H225" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I225" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>45</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E226" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="H226" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I226" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>45</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E227" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F227" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="H227" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I227" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>45</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="E228" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="H228" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I228" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>45</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E229" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="F229" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H229" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I229" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>45</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="H230" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I230" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>45</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E231" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G231" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H231" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I231" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>45</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E232" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H232" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I232" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>45</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F233" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="H233" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I233" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>45</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F234" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H234" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I234" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>45</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="F235" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="H235" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I235" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>45</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="H236" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I236" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>45</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E237" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="H237" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I237" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>45</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D238" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="E238" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H238" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I238" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>45</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E239" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="H239" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I239" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>45</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E240" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H240" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I240" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>45</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E241" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="F241" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="H241" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I241" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>45</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F242" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="H242" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I242" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>45</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E243" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H243" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I243" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>45</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="E244" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H244" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I244" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>45</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E245" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="H245" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I245" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>45</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E246" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="F246" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="H246" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I246" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>45</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C247" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="E247" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F247" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="H247" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I247" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>45</v>
+      </c>
+      <c r="B248" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C248" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D248" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="H248" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I248" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>45</v>
+      </c>
+      <c r="B249" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D249" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E249" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F249" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H249" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I249" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>45</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D250" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E250" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="F250" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H250" s="4">
+        <v>43369</v>
+      </c>
+      <c r="I250" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>45</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="D251" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E251" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="H251" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I251" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>45</v>
+      </c>
+      <c r="B252" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D252" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E252" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="H252" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I252" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>45</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D253" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E253" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F253" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G253" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H253" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I253" s="2">
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualización EXCEL Horarios de Cursada 2do Cuatrimestre 2018
</commit_message>
<xml_diff>
--- a/03. Analisis y diseño/04. Base de datos/04. Archivos/tempus_mesas_sep18.xlsx
+++ b/03. Analisis y diseño/04. Base de datos/04. Archivos/tempus_mesas_sep18.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="436">
   <si>
     <t>Matemática I</t>
   </si>
@@ -1232,6 +1232,96 @@
   </si>
   <si>
     <t>Tecnicatura Universitaria En Turismo</t>
+  </si>
+  <si>
+    <t>Planificacion I</t>
+  </si>
+  <si>
+    <t>Planificacion II</t>
+  </si>
+  <si>
+    <t>Taller De Integracion I</t>
+  </si>
+  <si>
+    <t>Teoria Politica</t>
+  </si>
+  <si>
+    <t>Metodologia De La Investigacion I</t>
+  </si>
+  <si>
+    <t>Metodologia De La Investigacion II</t>
+  </si>
+  <si>
+    <t>Politicas Publicas</t>
+  </si>
+  <si>
+    <t>Introduccion A Las Ciencias Sociales</t>
+  </si>
+  <si>
+    <t>Zubimendi</t>
+  </si>
+  <si>
+    <t>Ramirez S.</t>
+  </si>
+  <si>
+    <t>Lopez D.</t>
+  </si>
+  <si>
+    <t>Britos A.</t>
+  </si>
+  <si>
+    <t>Mocca J.</t>
+  </si>
+  <si>
+    <t>Escobar R.</t>
+  </si>
+  <si>
+    <t>Perez I.</t>
+  </si>
+  <si>
+    <t>Taller De Integracion III</t>
+  </si>
+  <si>
+    <t>Licenciatura En Trabajo Social</t>
+  </si>
+  <si>
+    <t>Desarrollo Local Y Economia Social</t>
+  </si>
+  <si>
+    <t>Fund. Y Const. Historica Del Trabajo Social</t>
+  </si>
+  <si>
+    <t>Taller De Integracion VIII</t>
+  </si>
+  <si>
+    <t>Teoria De La Intervencion Social</t>
+  </si>
+  <si>
+    <t>Instrumentos De Intervacion I</t>
+  </si>
+  <si>
+    <t>Practica I Diagnostico</t>
+  </si>
+  <si>
+    <t>Practica III Evaluacion</t>
+  </si>
+  <si>
+    <t>El Derecho Y La Conformacion De Las Instituciones</t>
+  </si>
+  <si>
+    <t>Sujeto Psicosocial Y Desarrollo Humano</t>
+  </si>
+  <si>
+    <t>Bustamante H.</t>
+  </si>
+  <si>
+    <t>Aveldaño A.</t>
+  </si>
+  <si>
+    <t>Are M.</t>
+  </si>
+  <si>
+    <t>Tenaglia M.</t>
   </si>
 </sst>
 </file>
@@ -1577,22 +1667,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I253"/>
+  <dimension ref="A1:I276"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B253" sqref="B253"/>
+    <sheetView tabSelected="1" topLeftCell="A280" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B257" sqref="B257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -8118,6 +8208,575 @@
         <v>0.625</v>
       </c>
     </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>74</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C254" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D254" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E254" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F254" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H254" s="1">
+        <v>43367</v>
+      </c>
+      <c r="I254" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>74</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D255" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E255" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F255" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H255" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I255" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>74</v>
+      </c>
+      <c r="B256" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D256" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E256" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F256" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H256" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I256" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>74</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D257" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="E257" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="F257" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="H257" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I257" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>74</v>
+      </c>
+      <c r="B258" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C258" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D258" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="E258" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="F258" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="H258" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I258" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>74</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C259" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D259" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E259" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H259" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I259" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>74</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D260" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E260" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="H260" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I260" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>74</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D261" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E261" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H261" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I261" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>74</v>
+      </c>
+      <c r="B262" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D262" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="E262" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="F262" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H262" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I262" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>74</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="D263" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="E263" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="F263" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H263" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I263" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>74</v>
+      </c>
+      <c r="B264" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D264" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="E264" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="F264" s="3"/>
+      <c r="H264" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I264" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>74</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D265" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E265" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="H265" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I265" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>74</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D266" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E266" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F266" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="H266" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I266" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>74</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C267" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D267" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E267" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H267" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I267" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>74</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C268" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="D268" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E268" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F268" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="H268" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I268" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>74</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E269" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="H269" s="1">
+        <v>43370</v>
+      </c>
+      <c r="I269" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>74</v>
+      </c>
+      <c r="B270" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C270" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D270" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E270" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="F270" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="H270" s="1">
+        <v>43371</v>
+      </c>
+      <c r="I270" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>74</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C271" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="D271" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E271" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="H271" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I271" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>74</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C272" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="D272" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E272" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="H272" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I272" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>74</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D273" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E273" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="F273" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="H273" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I273" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>74</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C274" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D274" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E274" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="F274" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="H274" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I274" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>74</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C275" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E275" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="F275" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H275" s="1">
+        <v>43368</v>
+      </c>
+      <c r="I275" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>74</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="D276" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="E276" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="H276" s="1">
+        <v>43369</v>
+      </c>
+      <c r="I276" s="2">
+        <v>0.75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>